<commit_message>
Moved the memory location of snake body in SNAKE_GAME.mips. Also changed the I/O portal memory location. Working on tetris dunno if possible to implement in 256 instruction memory :(.
</commit_message>
<xml_diff>
--- a/Control Mappings.xlsx
+++ b/Control Mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSE_CourseMaterials\CSES 210 - ARCHITECTURE SESSIONAL\MIPS_Assignment_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DE131E-A96A-4E1A-9655-73597FC4ACB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159B8BC0-2ED7-4BC3-82F2-CB49E76F32C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
   <si>
     <t>Binary</t>
   </si>
@@ -207,33 +207,18 @@
     <t>DATA + STACK</t>
   </si>
   <si>
-    <t>#ff</t>
-  </si>
-  <si>
     <t>Memory Layout Mapping (Binary)</t>
   </si>
   <si>
     <t>I/O PERIPHERAL</t>
   </si>
   <si>
-    <t>#af</t>
-  </si>
-  <si>
-    <t>SNAKE BODY</t>
-  </si>
-  <si>
     <t>FROM</t>
   </si>
   <si>
     <t>TO</t>
   </si>
   <si>
-    <t>#c0</t>
-  </si>
-  <si>
-    <t>#a0</t>
-  </si>
-  <si>
     <t>Decimal</t>
   </si>
   <si>
@@ -264,10 +249,19 @@
     <t>$io</t>
   </si>
   <si>
-    <t>EXTENDED MIPS WITH IO PERIPHERAL (for snake game)</t>
-  </si>
-  <si>
     <t>update these columns if series changes (according to group)</t>
+  </si>
+  <si>
+    <t>#F0</t>
+  </si>
+  <si>
+    <t>#FF</t>
+  </si>
+  <si>
+    <t>#EF</t>
+  </si>
+  <si>
+    <t>EXTENDED MIPS WITH IO PERIPHERAL</t>
   </si>
 </sst>
 </file>
@@ -402,6 +396,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -409,15 +412,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AH26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="104" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,11 +762,11 @@
       <c r="O2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
       <c r="S2" s="1" t="s">
         <v>31</v>
       </c>
@@ -782,12 +776,12 @@
       <c r="U2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="X2" s="13"/>
+      <c r="X2" s="15"/>
       <c r="Z2" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AA2" s="16"/>
       <c r="AB2" s="16"/>
@@ -880,10 +874,10 @@
       <c r="X3" s="10">
         <v>0</v>
       </c>
-      <c r="AG3" s="13" t="s">
+      <c r="AG3" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="AH3" s="13"/>
+      <c r="AH3" s="15"/>
     </row>
     <row r="4" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B4">
@@ -967,11 +961,11 @@
       <c r="X4" s="10">
         <v>1</v>
       </c>
-      <c r="Z4" s="13" t="s">
+      <c r="Z4" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="13"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
       <c r="AG4" t="s">
         <v>53</v>
       </c>
@@ -1159,11 +1153,11 @@
       <c r="X6" s="10">
         <v>11</v>
       </c>
-      <c r="Z6" s="11" t="s">
+      <c r="Z6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AA6" s="11" t="s">
-        <v>63</v>
+      <c r="AA6" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="AB6" s="11" t="s">
         <v>59</v>
@@ -1257,14 +1251,14 @@
       <c r="X7" s="10">
         <v>100</v>
       </c>
-      <c r="Z7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>63</v>
+      <c r="Z7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA7" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="AB7" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AG7" t="s">
         <v>50</v>
@@ -1355,15 +1349,6 @@
       <c r="X8" s="10">
         <v>101</v>
       </c>
-      <c r="Z8" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA8" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="AG8" t="s">
         <v>51</v>
       </c>
@@ -1619,12 +1604,12 @@
         <f t="shared" ca="1" si="14"/>
         <v>C40</v>
       </c>
-      <c r="W11" s="13" t="s">
+      <c r="W11" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="X11" s="13"/>
+      <c r="X11" s="15"/>
       <c r="AG11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="AH11" s="10">
         <v>111</v>
@@ -1706,14 +1691,14 @@
         <f t="shared" ca="1" si="14"/>
         <v>501</v>
       </c>
-      <c r="W12" s="18">
+      <c r="W12" s="14">
         <v>0</v>
       </c>
       <c r="X12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="AG12" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="AH12" s="10">
         <v>1000</v>
@@ -1795,14 +1780,14 @@
         <f t="shared" ca="1" si="14"/>
         <v>500</v>
       </c>
-      <c r="W13" s="18">
+      <c r="W13" s="14">
         <v>1</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="AG13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="AH13" s="10">
         <v>1001</v>
@@ -1884,23 +1869,23 @@
         <f t="shared" ca="1" si="14"/>
         <v>505</v>
       </c>
-      <c r="W14" s="18">
+      <c r="W14" s="14">
         <v>10</v>
       </c>
       <c r="X14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Z14" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA14" s="13"/>
-      <c r="AB14" s="13"/>
-      <c r="AD14" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE14" s="13"/>
-      <c r="AG14" s="17" t="s">
-        <v>73</v>
+      <c r="Z14" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AD14" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE14" s="15"/>
+      <c r="AG14" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="AH14" s="10">
         <v>1010</v>
@@ -1982,7 +1967,7 @@
         <f t="shared" ca="1" si="14"/>
         <v>900</v>
       </c>
-      <c r="W15" s="18">
+      <c r="W15" s="14">
         <v>11</v>
       </c>
       <c r="X15" s="1" t="s">
@@ -1998,13 +1983,13 @@
         <v>1</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AG15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="AH15" s="10">
         <v>1011</v>
@@ -2086,7 +2071,7 @@
         <f t="shared" ca="1" si="14"/>
         <v>780</v>
       </c>
-      <c r="W16" s="18">
+      <c r="W16" s="14">
         <v>100</v>
       </c>
       <c r="X16" s="1" t="s">
@@ -2098,21 +2083,21 @@
       </c>
       <c r="AA16" s="12" t="str">
         <f>DEC2BIN(HEX2DEC(MID(AA6, 2, LEN(AA6))))</f>
-        <v>10101111</v>
+        <v>11101111</v>
       </c>
       <c r="AB16" s="11" t="s">
         <v>59</v>
       </c>
       <c r="AD16">
-        <f t="shared" ref="AD16:AD18" ca="1" si="15">SUMPRODUCT(MID(Z16,LEN(Z16)-ROW(INDIRECT("1:"&amp;LEN(Z16)))+1,1)*2^(ROW(INDIRECT("1:"&amp;LEN(Z16)))-1))</f>
+        <f ca="1">SUMPRODUCT(MID(Z16,LEN(Z16)-ROW(INDIRECT("1:"&amp;LEN(Z16)))+1,1)*2^(ROW(INDIRECT("1:"&amp;LEN(Z16)))-1))</f>
         <v>0</v>
       </c>
       <c r="AE16">
         <f ca="1">SUMPRODUCT(MID(AA16,LEN(AA16)-ROW(INDIRECT("1:"&amp;LEN(AA16)))+1,1)*2^(ROW(INDIRECT("1:"&amp;LEN(AA16)))-1))</f>
-        <v>175</v>
+        <v>239</v>
       </c>
       <c r="AG16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AH16" s="10">
         <v>1100</v>
@@ -2194,33 +2179,33 @@
         <f t="shared" ca="1" si="14"/>
         <v>902</v>
       </c>
-      <c r="W17" s="18">
+      <c r="W17" s="14">
         <v>101</v>
       </c>
       <c r="X17" s="1" t="s">
         <v>28</v>
       </c>
       <c r="Z17" s="12" t="str">
-        <f t="shared" ref="Z17:AA18" si="16">DEC2BIN(HEX2DEC(MID(Z7, 2, LEN(Z7))))</f>
-        <v>10100000</v>
+        <f>DEC2BIN(HEX2DEC(MID(Z7, 2, LEN(Z7))))</f>
+        <v>11110000</v>
       </c>
       <c r="AA17" s="12" t="str">
-        <f t="shared" si="16"/>
-        <v>10101111</v>
+        <f>DEC2BIN(HEX2DEC(MID(AA7, 2, LEN(AA7))))</f>
+        <v>11111111</v>
       </c>
       <c r="AB17" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD17">
-        <f t="shared" ca="1" si="15"/>
-        <v>160</v>
+        <f t="shared" ref="AD16:AD18" ca="1" si="15">SUMPRODUCT(MID(Z17,LEN(Z17)-ROW(INDIRECT("1:"&amp;LEN(Z17)))+1,1)*2^(ROW(INDIRECT("1:"&amp;LEN(Z17)))-1))</f>
+        <v>240</v>
       </c>
       <c r="AE17">
-        <f t="shared" ref="AE17:AE18" ca="1" si="17">SUMPRODUCT(MID(AA17,LEN(AA17)-ROW(INDIRECT("1:"&amp;LEN(AA17)))+1,1)*2^(ROW(INDIRECT("1:"&amp;LEN(AA17)))-1))</f>
-        <v>175</v>
+        <f t="shared" ref="AE17:AE18" ca="1" si="16">SUMPRODUCT(MID(AA17,LEN(AA17)-ROW(INDIRECT("1:"&amp;LEN(AA17)))+1,1)*2^(ROW(INDIRECT("1:"&amp;LEN(AA17)))-1))</f>
+        <v>255</v>
       </c>
       <c r="AG17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="AH17" s="10">
         <v>1101</v>
@@ -2302,57 +2287,41 @@
         <f t="shared" ca="1" si="14"/>
         <v>8</v>
       </c>
-      <c r="W18" s="18">
+      <c r="W18" s="14">
         <v>110</v>
       </c>
       <c r="X18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Z18" s="12" t="str">
-        <f t="shared" si="16"/>
-        <v>11000000</v>
-      </c>
-      <c r="AA18" s="12" t="str">
-        <f t="shared" si="16"/>
-        <v>11111111</v>
-      </c>
-      <c r="AB18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD18">
-        <f t="shared" ca="1" si="15"/>
-        <v>192</v>
-      </c>
-      <c r="AE18">
-        <f t="shared" ca="1" si="17"/>
-        <v>255</v>
-      </c>
+      <c r="Z18" s="12"/>
+      <c r="AA18" s="12"/>
+      <c r="AB18" s="2"/>
       <c r="AG18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AH18" s="10">
         <v>1110</v>
       </c>
     </row>
     <row r="19" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="W19" s="18">
+      <c r="W19" s="14">
         <v>111</v>
       </c>
       <c r="X19" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AG19" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AH19" s="10">
         <v>1111</v>
       </c>
     </row>
     <row r="20" spans="2:34" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="15"/>
+      <c r="E20" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="18"/>
       <c r="U20" s="8" t="str">
         <f ca="1">_xlfn.CONCAT("v2.0 raw", CHAR(10), _xlfn.TEXTJOIN(" ", TRUE, U3:U18))</f>
         <v>v2.0 raw
@@ -2366,86 +2335,86 @@
       </c>
     </row>
     <row r="23" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
       <c r="U23" s="6"/>
     </row>
     <row r="25" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
     </row>
     <row r="26" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="B26:S26"/>
+    <mergeCell ref="B23:S23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:S25"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="AG3:AH3"/>
     <mergeCell ref="Z2:AH2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="Z14:AB14"/>
     <mergeCell ref="W11:X11"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="B26:S26"/>
-    <mergeCell ref="B23:S23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:S25"/>
-    <mergeCell ref="E20:F20"/>
     <mergeCell ref="AD14:AE14"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>